<commit_message>
adding all code and related folders
</commit_message>
<xml_diff>
--- a/Assignment 2/gutenbergGraphs.xlsx
+++ b/Assignment 2/gutenbergGraphs.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="bryant-stories.txt" sheetId="1" r:id="rId1"/>
+    <sheet name="carroll-alice.txt" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -109,7 +109,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="bryant-stories.txtfig1.jpeg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="carroll-alice.txtfig1.jpeg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -147,7 +147,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="bryant-stories.txtfig2.jpeg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="carroll-alice.txtfig2.jpeg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>

<commit_message>
adding all the mentioned files
</commit_message>
<xml_diff>
--- a/Assignment 2/gutenbergGraphs.xlsx
+++ b/Assignment 2/gutenbergGraphs.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="carroll-alice.txt" sheetId="1" r:id="rId1"/>
+    <sheet name="blake-poems.txt" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -109,7 +109,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="carroll-alice.txtfig1.jpeg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="blake-poems.txtfig1.jpeg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -147,7 +147,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="carroll-alice.txtfig2.jpeg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="blake-poems.txtfig2.jpeg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>